<commit_message>
Actually reformat numbers according to their format in Spreadsheet::Read
This still is horribly hacky but works for my purposes. Ideally, later
I will do a feature-based implementation instead of per-parser hacks, but
maybe this even needs to remain per-parser.

Still, making those hacks configurable would be nice.
</commit_message>
<xml_diff>
--- a/t/Accounting-test.xlsx
+++ b/t/Accounting-test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Invoices" sheetId="1" state="visible" r:id="rId2"/>
@@ -276,7 +276,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
   </numFmts>
@@ -637,24 +637,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,21 +830,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,7 +891,8 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0</v>
+        <f aca="false">C2*1.19</f>
+        <v>4760</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>28</v>
@@ -974,7 +970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -984,10 +980,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1100,7 +1093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1110,10 +1103,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>